<commit_message>
PF ini generation number auto + matplotlib version
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7362815-790A-4825-9E28-6BEDA0B66DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC70114-FB3A-4CCD-B62E-D17174D80888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
     <sheet name="map" sheetId="6" r:id="rId2"/>
-    <sheet name="map (2)" sheetId="7" r:id="rId3"/>
-    <sheet name="map (4)" sheetId="9" r:id="rId4"/>
-    <sheet name="map (5)" sheetId="10" r:id="rId5"/>
+    <sheet name="map (1)" sheetId="11" r:id="rId3"/>
+    <sheet name="map (2)" sheetId="7" r:id="rId4"/>
+    <sheet name="map (4)" sheetId="9" r:id="rId5"/>
+    <sheet name="map (5)" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>Composants</t>
   </si>
@@ -280,6 +281,15 @@
   </si>
   <si>
     <t>E7</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -644,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1363,11 +1373,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C3ECA9-050A-4ABB-904A-776388DE759D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66F79B1-DCBF-4D89-8213-78C4884EC29A}">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -1428,25 +1438,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1484,11 +1494,11 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
+      <c r="B5" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1496,8 +1506,8 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
+      <c r="F5" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -1521,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1566,16 +1576,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1626,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1656,6 +1666,299 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C3ECA9-050A-4ABB-904A-776388DE759D}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="5.28515625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F848A8BD-D29C-4474-9AF8-726898719083}">
   <dimension ref="A1:O20"/>
   <sheetViews>
@@ -2626,12 +2929,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAD7F43-4D99-46C4-B1C7-A2E91585DDA9}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2909,8 +3212,8 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>76</v>
+      <c r="P5" s="2">
+        <v>0</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
PF wall & rename app
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC70114-FB3A-4CCD-B62E-D17174D80888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A6EC51-66F5-4FBF-BC0A-1EC2044957E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
     <sheet name="map" sheetId="6" r:id="rId2"/>
     <sheet name="map (1)" sheetId="11" r:id="rId3"/>
-    <sheet name="map (2)" sheetId="7" r:id="rId4"/>
+    <sheet name="map (2)" sheetId="12" r:id="rId4"/>
     <sheet name="map (4)" sheetId="9" r:id="rId5"/>
-    <sheet name="map (5)" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>Composants</t>
   </si>
@@ -229,58 +228,10 @@
     <t>E0</t>
   </si>
   <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>E7</t>
   </si>
   <si>
     <t>C</t>
@@ -1034,7 +985,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1059,7 +1010,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1377,7 +1328,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1348,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -1438,25 +1389,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1495,10 +1446,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1506,8 +1457,8 @@
       <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>82</v>
+      <c r="F5" s="2">
+        <v>0</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
@@ -1531,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1575,17 +1526,17 @@
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>82</v>
+      <c r="B8" s="2">
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1636,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1666,11 +1617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C3ECA9-050A-4ABB-904A-776388DE759D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EADA6D6B-ABA7-483C-BECD-8EB537192F5F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2">
         <v>1</v>
@@ -1731,25 +1682,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1770,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1787,11 +1738,11 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
+      <c r="B5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1818,13 +1769,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -1868,17 +1819,17 @@
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>60</v>
+      <c r="B8" s="2">
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1929,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1963,7 +1914,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,13 +1931,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2">
         <v>1</v>
@@ -2004,13 +1955,13 @@
         <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>64</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="2">
         <v>1</v>
@@ -2162,20 +2113,20 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
@@ -2189,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -2204,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2336,7 +2287,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
@@ -2383,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -2491,7 +2442,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
@@ -2500,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -2518,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -2533,7 +2484,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2738,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -2753,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K17" s="2">
         <v>0</v>
@@ -2876,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
@@ -2897,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="L20" s="2">
         <v>1</v>
@@ -2927,1106 +2878,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAD7F43-4D99-46C4-B1C7-A2E91585DDA9}">
-  <dimension ref="A1:Q20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="2">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2">
-        <v>1</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="2">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2">
-        <v>1</v>
-      </c>
-      <c r="P1" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0</v>
-      </c>
-      <c r="O19" s="2">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" s="2">
-        <v>1</v>
-      </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
-      <c r="O20" s="2">
-        <v>1</v>
-      </c>
-      <c r="P20" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:Q20">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Pompe feature P1 & P3
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A6EC51-66F5-4FBF-BC0A-1EC2044957E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF5498-103B-4278-BD0A-55426336D78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,9 +709,15 @@
         <v>41</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="H3" s="5">
+        <v>-5.1599999999999997E-4</v>
+      </c>
+      <c r="I3" s="5">
+        <v>-1.54E-2</v>
+      </c>
+      <c r="J3" s="6">
+        <v>4.87</v>
+      </c>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1620,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EADA6D6B-ABA7-483C-BECD-8EB537192F5F}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1914,7 +1920,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,13 +2181,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -2222,13 +2228,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -2269,13 +2275,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
refacto group & widget
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BF5498-103B-4278-BD0A-55426336D78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6DF3A-CB50-4072-9D50-19F1799884D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,9 @@
       <c r="F3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
       <c r="H3" s="5">
         <v>-5.1599999999999997E-4</v>
       </c>

</xml_diff>

<commit_message>
Pc auto & durites
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858AA140-1564-405E-BF7D-C63A0111C70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4CCC7F-FA5C-4FCA-BDDD-09A1D1D13925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
     <sheet name="map" sheetId="6" r:id="rId2"/>
     <sheet name="map (2)" sheetId="9" r:id="rId3"/>
+    <sheet name="lines" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>Composants</t>
   </si>
@@ -175,12 +176,6 @@
     <t>Eb</t>
   </si>
   <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>Tb</t>
-  </si>
-  <si>
     <t>Ra</t>
   </si>
   <si>
@@ -239,6 +234,69 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>durite</t>
+  </si>
+  <si>
+    <t>E0-C0</t>
+  </si>
+  <si>
+    <t>E0-C1</t>
+  </si>
+  <si>
+    <t>E0-C2</t>
+  </si>
+  <si>
+    <t>E0-C3</t>
+  </si>
+  <si>
+    <t>P0-E0</t>
+  </si>
+  <si>
+    <t>P1-E0</t>
+  </si>
+  <si>
+    <t>E1-C0</t>
+  </si>
+  <si>
+    <t>E1-C1</t>
+  </si>
+  <si>
+    <t>E1-C2</t>
+  </si>
+  <si>
+    <t>E1-C3</t>
+  </si>
+  <si>
+    <t>P0-E1</t>
+  </si>
+  <si>
+    <t>P1-E1</t>
+  </si>
+  <si>
+    <t>E2-C0</t>
+  </si>
+  <si>
+    <t>E2-C1</t>
+  </si>
+  <si>
+    <t>E2-C2</t>
+  </si>
+  <si>
+    <t>E2-C3</t>
+  </si>
+  <si>
+    <t>P0-E2</t>
+  </si>
+  <si>
+    <t>P1-E2</t>
   </si>
 </sst>
 </file>
@@ -248,7 +306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +319,14 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -277,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -300,11 +366,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,6 +401,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,12 +690,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.85546875" style="2"/>
     <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -645,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>35</v>
@@ -662,7 +744,7 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -698,7 +780,7 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -734,7 +816,7 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -770,7 +852,7 @@
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -802,7 +884,7 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -830,7 +912,7 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -848,8 +930,8 @@
       <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>45</v>
+      <c r="G7" s="3">
+        <v>4</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -862,7 +944,7 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -880,8 +962,8 @@
       <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>46</v>
+      <c r="G8" s="3">
+        <v>8</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -894,7 +976,7 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -920,7 +1002,7 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -937,7 +1019,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -950,7 +1032,7 @@
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -967,7 +1049,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="6"/>
@@ -976,7 +1058,7 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -993,7 +1075,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="6"/>
@@ -1002,7 +1084,7 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1019,7 +1101,7 @@
         <v>40</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="6"/>
@@ -1028,11 +1110,11 @@
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>33</v>
@@ -1041,7 +1123,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1056,11 +1138,11 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>34</v>
@@ -1069,7 +1151,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -1140,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1187,25 +1269,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1289,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -1340,10 +1422,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1406,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1507,13 +1589,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -1531,13 +1613,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -1701,20 +1783,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
@@ -1728,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
@@ -1743,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2051,20 +2133,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="G13" s="2">
         <v>0</v>
       </c>
@@ -2078,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L13" s="2">
         <v>0</v>
@@ -2093,7 +2175,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2313,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -2328,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -2460,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -2481,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -2511,4 +2593,285 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83EA192-CDD2-433B-90DB-5911726BE736}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15">
+        <v>0.7</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel & widget refacto nature0 groupe0 & limite0
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4CCC7F-FA5C-4FCA-BDDD-09A1D1D13925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0168A441-E4D2-4CFF-92D7-440691627FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="map" sheetId="6" r:id="rId2"/>
     <sheet name="map (2)" sheetId="9" r:id="rId3"/>
     <sheet name="lines" sheetId="10" r:id="rId4"/>
+    <sheet name="slot" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
   <si>
     <t>Composants</t>
   </si>
@@ -297,6 +298,18 @@
   </si>
   <si>
     <t>P1-E2</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>capteur</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>limit</t>
   </si>
 </sst>
 </file>
@@ -2600,11 +2613,12 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
@@ -2623,10 +2637,10 @@
       <c r="A2" s="8">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.3</v>
       </c>
       <c r="D2" s="2">
@@ -2637,10 +2651,10 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.6</v>
       </c>
       <c r="D3" s="2">
@@ -2651,10 +2665,10 @@
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.2</v>
       </c>
       <c r="D4" s="2">
@@ -2665,10 +2679,10 @@
       <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.8</v>
       </c>
       <c r="D5" s="2">
@@ -2679,10 +2693,10 @@
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.2</v>
       </c>
       <c r="D6" s="2">
@@ -2693,10 +2707,10 @@
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.8</v>
       </c>
       <c r="D7" s="2">
@@ -2707,10 +2721,10 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.6</v>
       </c>
       <c r="D8" s="2">
@@ -2721,10 +2735,10 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.7</v>
       </c>
       <c r="D9" s="2">
@@ -2735,10 +2749,10 @@
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.5</v>
       </c>
       <c r="D10" s="2">
@@ -2749,10 +2763,10 @@
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.5</v>
       </c>
       <c r="D11" s="2">
@@ -2763,24 +2777,24 @@
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C12">
-        <v>0.5</v>
+      <c r="C12" s="2">
+        <v>0.1</v>
       </c>
       <c r="D12" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.5</v>
       </c>
       <c r="D13" s="2">
@@ -2791,10 +2805,10 @@
       <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.8</v>
       </c>
       <c r="D14" s="2">
@@ -2805,10 +2819,10 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.7</v>
       </c>
       <c r="D15" s="2">
@@ -2819,10 +2833,10 @@
       <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.9</v>
       </c>
       <c r="D16" s="2">
@@ -2833,10 +2847,10 @@
       <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>0.3</v>
       </c>
       <c r="D17" s="2">
@@ -2847,10 +2861,10 @@
       <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>0.5</v>
       </c>
       <c r="D18" s="2">
@@ -2861,14 +2875,114 @@
       <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.1</v>
       </c>
       <c r="D19" s="2">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7F672C-2A39-4AB6-AF2E-4F855F1E37BE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug init dfcapteur &  limit = float
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0168A441-E4D2-4CFF-92D7-440691627FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5569B258-3BB0-4E63-B4B4-4B250FD99E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="4188" windowWidth="46080" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
     <sheet name="map" sheetId="6" r:id="rId2"/>
     <sheet name="map (2)" sheetId="9" r:id="rId3"/>
-    <sheet name="lines" sheetId="10" r:id="rId4"/>
-    <sheet name="slot" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>Composants</t>
   </si>
@@ -235,81 +233,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>dist</t>
-  </si>
-  <si>
-    <t>durite</t>
-  </si>
-  <si>
-    <t>E0-C0</t>
-  </si>
-  <si>
-    <t>E0-C1</t>
-  </si>
-  <si>
-    <t>E0-C2</t>
-  </si>
-  <si>
-    <t>E0-C3</t>
-  </si>
-  <si>
-    <t>P0-E0</t>
-  </si>
-  <si>
-    <t>P1-E0</t>
-  </si>
-  <si>
-    <t>E1-C0</t>
-  </si>
-  <si>
-    <t>E1-C1</t>
-  </si>
-  <si>
-    <t>E1-C2</t>
-  </si>
-  <si>
-    <t>E1-C3</t>
-  </si>
-  <si>
-    <t>P0-E1</t>
-  </si>
-  <si>
-    <t>P1-E1</t>
-  </si>
-  <si>
-    <t>E2-C0</t>
-  </si>
-  <si>
-    <t>E2-C1</t>
-  </si>
-  <si>
-    <t>E2-C2</t>
-  </si>
-  <si>
-    <t>E2-C3</t>
-  </si>
-  <si>
-    <t>P0-E2</t>
-  </si>
-  <si>
-    <t>P1-E2</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>capteur</t>
-  </si>
-  <si>
-    <t>nature</t>
-  </si>
-  <si>
-    <t>limit</t>
   </si>
 </sst>
 </file>
@@ -319,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,14 +255,6 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -356,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -379,20 +294,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -414,12 +320,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,20 +607,20 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>39</v>
       </c>
@@ -756,7 +656,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -792,7 +692,7 @@
       </c>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -828,7 +728,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -864,7 +764,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -896,7 +796,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -924,7 +824,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -956,7 +856,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -988,7 +888,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1014,7 +914,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1044,7 +944,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1070,7 +970,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1096,7 +996,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1122,7 +1022,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1150,7 +1050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1192,13 +1092,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="8" width="5.28515625" style="2" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="2"/>
+    <col min="2" max="8" width="5.33203125" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -1221,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1247,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1277,7 +1177,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1307,7 +1207,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1337,7 +1237,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1367,7 +1267,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1397,7 +1297,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1427,7 +1327,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1457,7 +1357,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1487,7 +1387,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1534,17 +1434,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F848A8BD-D29C-4474-9AF8-726898719083}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="11" width="3.85546875" style="2" customWidth="1"/>
-    <col min="12" max="16" width="3.85546875" customWidth="1"/>
+    <col min="2" max="11" width="3.88671875" style="2" customWidth="1"/>
+    <col min="12" max="16" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -1591,7 +1491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1641,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1691,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1741,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1791,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1841,7 +1741,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1891,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1941,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1991,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2041,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2091,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2141,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2191,7 +2091,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2241,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2291,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2341,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2391,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2441,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2491,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2541,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2606,386 +2506,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83EA192-CDD2-433B-90DB-5911726BE736}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="8.85546875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="D15" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="D16" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="D17" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7F672C-2A39-4AB6-AF2E-4F855F1E37BE}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
BUS v1 debit & masse cout durite
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bertrand\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5569B258-3BB0-4E63-B4B4-4B250FD99E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65B7A1A-B27C-4848-8D14-D7C1E3A01BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="4188" windowWidth="46080" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Composants</t>
   </si>
@@ -191,33 +191,6 @@
   </si>
   <si>
     <t>Actif</t>
-  </si>
-  <si>
-    <t>C0</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>P0</t>
-  </si>
-  <si>
-    <t>E0</t>
   </si>
   <si>
     <t>F</t>
@@ -607,20 +580,20 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>39</v>
       </c>
@@ -656,7 +629,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -692,7 +665,7 @@
       </c>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -728,7 +701,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -764,7 +737,7 @@
       </c>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -796,7 +769,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -824,7 +797,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -856,7 +829,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -888,7 +861,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -914,7 +887,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -944,7 +917,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -970,7 +943,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -996,7 +969,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1022,7 +995,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1036,7 +1009,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1050,7 +1023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1064,7 +1037,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -1088,17 +1061,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F29B31-6C0D-40B3-B31D-F123035F6D9E}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="5.33203125" style="2" customWidth="1"/>
-    <col min="9" max="11" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="8" width="5.28515625" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -1121,8 +1095,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2">
@@ -1135,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1147,8 +1121,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -1177,24 +1151,24 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -1207,8 +1181,8 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -1237,15 +1211,15 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
+      <c r="C6" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1267,8 +1241,8 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2">
@@ -1284,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -1297,8 +1271,8 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2">
@@ -1327,18 +1301,18 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1357,8 +1331,8 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2">
@@ -1387,8 +1361,8 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2">
@@ -1401,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1434,17 +1408,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F848A8BD-D29C-4474-9AF8-726898719083}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="3.88671875" style="2" customWidth="1"/>
-    <col min="12" max="16" width="3.88671875" customWidth="1"/>
+    <col min="2" max="11" width="3.85546875" style="2" customWidth="1"/>
+    <col min="12" max="16" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -1491,7 +1465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1502,13 +1476,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -1526,13 +1500,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -1541,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1591,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1641,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1691,12 +1665,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1705,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -1723,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
@@ -1738,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1791,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1841,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1891,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1941,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1991,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2041,12 +2015,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -2055,10 +2029,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -2073,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L13" s="2">
         <v>0</v>
@@ -2088,10 +2062,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2141,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2191,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2241,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2291,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2308,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -2323,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -2341,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2391,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2441,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2455,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -2476,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
correction bus group debit calcul
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD87A7D4-B248-45C7-AB26-8571025B13A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF4C7A-4AA3-4EA3-B749-8A34D16BE6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="46080" windowHeight="12120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69252" yWindow="2184" windowWidth="15324" windowHeight="12336" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="map s2" sheetId="12" r:id="rId4"/>
     <sheet name="map (2)" sheetId="9" r:id="rId5"/>
     <sheet name="map (3)" sheetId="10" r:id="rId6"/>
+    <sheet name="map T" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="57">
   <si>
     <t>Composants</t>
   </si>
@@ -209,6 +210,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -1758,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522EE95-236C-483A-8736-BE2CD2AF01BB}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1957,9 +1961,6 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="H7" s="2">
         <v>1</v>
       </c>
@@ -1975,8 +1976,8 @@
       <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3524,4 +3525,351 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939A697C-E35F-43C8-8BD2-E03FCDCB913A}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="8" width="5.33203125" style="2" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:H11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refacto import grid & size car
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59A5387-5CC3-44B0-92EF-15A817B0FC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449EDEC3-6B11-43DD-8E68-78D2F0AAE753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="88530" yWindow="5085" windowWidth="15030" windowHeight="10080" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="88950" yWindow="4440" windowWidth="15030" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -1515,7 +1515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF35672-D4E7-4E11-9F6D-AE904E9E6449}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC3C0F3-156C-44AC-8663-5C3D7F9A9281}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -3070,8 +3070,8 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
+      <c r="D5" s="2">
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -3100,8 +3100,8 @@
       <c r="C6" s="2">
         <v>0</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
+      <c r="D6" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
edited input & plot level
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449EDEC3-6B11-43DD-8E68-78D2F0AAE753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93223D1-6380-4358-B189-00B1349BD3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="88950" yWindow="4440" windowWidth="15030" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="30912" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="56">
   <si>
     <t>Composants</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>Pmin</t>
   </si>
   <si>
     <t>Categorie</t>
@@ -585,482 +582,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
+        <v>136</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>-5.1599999999999997E-4</v>
+      </c>
+      <c r="I2" s="5">
+        <v>-1.54E-2</v>
+      </c>
+      <c r="J2" s="6">
+        <v>4.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>130</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>-5.1599999999999997E-4</v>
+      </c>
+      <c r="I3" s="5">
+        <v>-1.54E-2</v>
+      </c>
+      <c r="J3" s="6">
+        <v>4.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>330</v>
+      </c>
+      <c r="E4" s="3">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>-6.6100000000000002E-4</v>
+      </c>
+      <c r="I4" s="6">
+        <v>-2.86E-2</v>
+      </c>
+      <c r="J4" s="5">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3">
+        <v>110</v>
+      </c>
+      <c r="E5" s="3">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3">
-        <v>136</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7.6400000000000003E-4</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3">
+        <v>150</v>
+      </c>
+      <c r="E6" s="3">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5">
-        <v>-5.1599999999999997E-4</v>
-      </c>
-      <c r="J2" s="5">
-        <v>-1.54E-2</v>
-      </c>
-      <c r="K2" s="6">
-        <v>4.87</v>
-      </c>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3">
-        <v>130</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5">
-        <v>-5.1599999999999997E-4</v>
-      </c>
-      <c r="J3" s="5">
-        <v>-1.54E-2</v>
-      </c>
-      <c r="K3" s="6">
-        <v>4.87</v>
-      </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3">
-        <v>330</v>
-      </c>
-      <c r="F4" s="3">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5">
-        <v>-6.6100000000000002E-4</v>
-      </c>
-      <c r="J4" s="6">
-        <v>-2.86E-2</v>
-      </c>
-      <c r="K4" s="5">
-        <v>12.1</v>
-      </c>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3">
-        <v>110</v>
-      </c>
-      <c r="F5" s="3">
-        <v>6</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
-        <v>7.6400000000000003E-4</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3">
-        <v>150</v>
-      </c>
-      <c r="F6" s="3">
-        <v>8</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="2">
-        <v>5</v>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2.3499999999999999E-4</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3">
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3">
-        <v>4</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2.3499999999999999E-4</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3">
+      <c r="D8" s="3">
         <v>83</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F8" s="3">
+        <v>8</v>
+      </c>
       <c r="G8" s="3">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <v>7.2000000000000005E-4</v>
       </c>
+      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="2">
-        <v>7</v>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>10</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="2">
-        <v>8</v>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <v>600</v>
+      </c>
+      <c r="E10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3">
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
         <v>600</v>
       </c>
-      <c r="F10" s="3">
-        <v>25</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="E11" s="3">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3">
-        <v>600</v>
-      </c>
-      <c r="F11" s="3">
-        <v>30</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="2">
-        <v>10</v>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
+        <v>600</v>
+      </c>
       <c r="E12" s="3">
-        <v>600</v>
-      </c>
-      <c r="F12" s="3">
         <v>35</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="2">
-        <v>11</v>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <v>600</v>
+      </c>
       <c r="E13" s="3">
-        <v>600</v>
-      </c>
-      <c r="F13" s="3">
         <v>40</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="2">
-        <v>12</v>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="F14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
+      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="2">
-        <v>13</v>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="F15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
         <v>1.6999999999999999E-3</v>
       </c>
+      <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1118,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1130,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -1153,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -1183,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -1201,13 +1132,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1225,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -1240,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1297,22 +1228,22 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1369,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1384,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1423,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1447,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1470,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1488,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -1583,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -1604,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -1683,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -1704,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -1777,7 +1708,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1804,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
@@ -1813,13 +1744,13 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -2036,25 +1967,25 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -2063,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O11" s="2">
         <v>0</v>
@@ -2127,7 +2058,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -2169,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2213,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -2377,13 +2308,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -2404,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -2419,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2536,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -2557,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -2647,7 +2578,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -2688,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -2700,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -2844,19 +2775,19 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2907,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -2940,7 +2871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC3C0F3-156C-44AC-8663-5C3D7F9A9281}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2994,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -3014,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -3050,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
@@ -3065,7 +2996,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -3101,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -3110,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -3155,13 +3086,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -3170,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -3251,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -3260,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
@@ -3329,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -3341,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -3382,25 +3313,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -3451,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -3475,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3502,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3529,25 +3460,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3598,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -3699,13 +3630,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -3723,13 +3654,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -3805,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -3879,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -3893,17 +3824,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
@@ -3935,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4243,20 +4174,20 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G13" s="2">
         <v>0</v>
       </c>
@@ -4279,13 +4210,13 @@
         <v>0</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O13" s="2">
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -4505,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -4520,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -4652,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -4673,7 +4604,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -4757,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -4804,25 +4735,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -4867,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -4906,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -4957,10 +4888,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -5023,7 +4954,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -5098,7 +5029,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5110,7 +5041,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -5151,25 +5082,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5220,7 +5151,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -5244,7 +5175,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -5280,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -5337,7 +5268,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -5364,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -5449,7 +5380,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5461,10 +5392,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
@@ -5484,7 +5415,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -5538,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5556,7 +5487,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -5568,7 +5499,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -5628,25 +5559,25 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5694,13 +5625,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -5718,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -5748,7 +5679,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -5772,7 +5703,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -5801,7 +5732,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -5816,7 +5747,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -5892,7 +5823,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5904,7 +5835,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -5960,7 +5891,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -5972,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -6002,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -6017,7 +5948,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -6047,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -6071,13 +6002,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -6119,7 +6050,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -6137,23 +6068,23 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
@@ -6161,7 +6092,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -6224,7 +6155,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -6244,7 +6175,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -6262,7 +6193,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
multiple correction / change
delete T0
check message update algo
fig + graph details
masse cout correction & split
!! optimisation graph T
clean params Tmode
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93223D1-6380-4358-B189-00B1349BD3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DACBA-378D-4F1F-A347-E10C343701B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="30912" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76680" yWindow="2610" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="50">
   <si>
     <t>Composants</t>
   </si>
@@ -138,15 +138,6 @@
     <t>1 Réservoir</t>
   </si>
   <si>
-    <t>2 Réservoirs</t>
-  </si>
-  <si>
-    <t>3 Réservoirs</t>
-  </si>
-  <si>
-    <t>4 Réservoirs</t>
-  </si>
-  <si>
     <t>Fixed</t>
   </si>
   <si>
@@ -181,15 +172,6 @@
   </si>
   <si>
     <t>Ra</t>
-  </si>
-  <si>
-    <t>Rb</t>
-  </si>
-  <si>
-    <t>Rc</t>
-  </si>
-  <si>
-    <t>Rd</t>
   </si>
   <si>
     <t>Nozzle</t>
@@ -582,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -602,7 +584,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -620,16 +602,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -650,7 +632,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -682,7 +664,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -714,7 +696,7 @@
         <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -746,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -774,10 +756,12 @@
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="6">
+        <v>7.6400000000000003E-4</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
@@ -874,7 +858,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -885,113 +869,47 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3">
-        <v>600</v>
-      </c>
-      <c r="E11" s="3">
-        <v>30</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3">
-        <v>600</v>
-      </c>
-      <c r="E12" s="3">
-        <v>35</v>
-      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <v>600</v>
-      </c>
-      <c r="E13" s="3">
-        <v>40</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="6">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1049,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1061,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -1084,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -1114,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -1132,13 +1050,13 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1156,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -1171,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1228,22 +1146,22 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
@@ -1300,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -1315,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
@@ -1354,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1378,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1401,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1419,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -1514,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -1535,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -1614,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -1635,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -1708,7 +1626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1735,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
@@ -1744,13 +1662,13 @@
         <v>0</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1967,25 +1885,25 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -1994,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="O11" s="2">
         <v>0</v>
@@ -2058,7 +1976,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -2100,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2144,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -2308,13 +2226,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -2335,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -2350,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2467,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -2488,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -2578,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -2619,7 +2537,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -2631,13 +2549,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -2775,19 +2693,19 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2838,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -2925,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -2945,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -2981,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
@@ -2996,7 +2914,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -3032,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -3041,7 +2959,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -3086,13 +3004,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -3101,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -3182,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -3191,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
@@ -3260,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -3272,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -3313,25 +3231,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -3382,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -3406,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3433,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3460,25 +3378,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3529,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -3630,13 +3548,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -3654,13 +3572,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
@@ -3736,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -3810,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -3824,7 +3742,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -3833,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -3866,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4174,7 +4092,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -4183,10 +4101,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -4210,13 +4128,13 @@
         <v>0</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O13" s="2">
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -4436,7 +4354,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -4451,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -4583,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
@@ -4604,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -4688,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -4735,25 +4653,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -4798,7 +4716,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -4837,7 +4755,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -4888,10 +4806,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -4954,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -5029,7 +4947,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5041,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -5082,25 +5000,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5151,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -5175,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -5211,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -5268,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -5295,7 +5213,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -5380,7 +5298,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5392,10 +5310,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
@@ -5415,7 +5333,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -5469,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5487,7 +5405,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -5499,7 +5417,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -5559,25 +5477,25 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5625,13 +5543,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -5649,7 +5567,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -5679,7 +5597,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -5703,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -5732,7 +5650,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -5747,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -5823,7 +5741,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -5835,7 +5753,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -5891,7 +5809,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -5903,7 +5821,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -5933,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -5948,7 +5866,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -5978,7 +5896,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -6002,13 +5920,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -6050,7 +5968,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -6068,13 +5986,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -6083,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
@@ -6092,7 +6010,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -6155,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -6175,7 +6093,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -6193,7 +6111,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>

</xml_diff>